<commit_message>
Added LDO for power off VSYS (to ensure enough current to LAN); Added datasheets for LDO and FTDI chip
</commit_message>
<xml_diff>
--- a/Hardware/v3/bom_v3.xlsx
+++ b/Hardware/v3/bom_v3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="226">
   <si>
     <t>Qty</t>
   </si>
@@ -626,13 +626,79 @@
   </si>
   <si>
     <t>CRYSTAL-ESC-32</t>
+  </si>
+  <si>
+    <t>1.0UF-16V-10%(0402)</t>
+  </si>
+  <si>
+    <t>0402-CAP</t>
+  </si>
+  <si>
+    <t>C20, C21</t>
+  </si>
+  <si>
+    <t>GRM155R60J105KE19D</t>
+  </si>
+  <si>
+    <t>490-1320-1-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/GRM155R60J105KE19D/490-1320-1-ND/587919</t>
+  </si>
+  <si>
+    <t>.1uF</t>
+  </si>
+  <si>
+    <t>0.1UF-16V(+-10%)(0402)</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>C1005X5R1H104K050BB</t>
+  </si>
+  <si>
+    <t>445-5942-1-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/C1005X5R1H104K050BB/445-5942-1-ND/2443982</t>
+  </si>
+  <si>
+    <t>MIC5353-XXYMT</t>
+  </si>
+  <si>
+    <t>MIC5353-3.3YMT</t>
+  </si>
+  <si>
+    <t>6-UFDFN</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>IC REG LDO 3.3V 0.5A 6TMLF</t>
+  </si>
+  <si>
+    <t>Micrel</t>
+  </si>
+  <si>
+    <t>MIC5353-3.3YMT TR</t>
+  </si>
+  <si>
+    <t>576-3680-1-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/MIC5353-3.3YMT%20TR/576-3680-1-ND/2339682</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -787,6 +853,19 @@
       <color rgb="FF333333"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1131,7 +1210,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1140,6 +1219,10 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="10"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="10" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1201,8 +1284,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="BOM" displayName="BOM" ref="A1:O27" totalsRowShown="0">
-  <autoFilter ref="A1:O27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="BOM" displayName="BOM" ref="A1:O30" totalsRowShown="0">
+  <autoFilter ref="A1:O30"/>
   <tableColumns count="15">
     <tableColumn id="1" name="Qty"/>
     <tableColumn id="2" name="Value"/>
@@ -1221,7 +1304,7 @@
       <calculatedColumnFormula>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="16" name="Final order qty" dataDxfId="0">
-      <calculatedColumnFormula>N30*BOM[[#This Row],[Qty]]</calculatedColumnFormula>
+      <calculatedColumnFormula>N32*BOM[[#This Row],[Qty]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1516,10 +1599,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:P31"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1625,7 +1708,7 @@
         <v>0.496</v>
       </c>
       <c r="O2">
-        <f>N30*BOM[[#This Row],[Qty]]</f>
+        <f>N32*BOM[[#This Row],[Qty]]</f>
         <v>10</v>
       </c>
     </row>
@@ -1668,7 +1751,7 @@
         <v>2E-3</v>
       </c>
       <c r="O3">
-        <f>N30*BOM[[#This Row],[Qty]]</f>
+        <f>N32*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -1711,7 +1794,7 @@
         <v>0.16200000000000001</v>
       </c>
       <c r="O4">
-        <f>N30*BOM[[#This Row],[Qty]]</f>
+        <f>N32*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -1754,7 +1837,7 @@
         <v>0.09</v>
       </c>
       <c r="O5">
-        <f>N30*BOM[[#This Row],[Qty]]</f>
+        <f>N32*BOM[[#This Row],[Qty]]</f>
         <v>75</v>
       </c>
     </row>
@@ -1797,7 +1880,7 @@
         <v>0.48</v>
       </c>
       <c r="O6">
-        <f>N30*BOM[[#This Row],[Qty]]</f>
+        <f>N32*BOM[[#This Row],[Qty]]</f>
         <v>10</v>
       </c>
     </row>
@@ -1840,7 +1923,7 @@
         <v>2E-3</v>
       </c>
       <c r="O7">
-        <f>N30*BOM[[#This Row],[Qty]]</f>
+        <f>N32*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -1883,7 +1966,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="O8">
-        <f>N30*BOM[[#This Row],[Qty]]</f>
+        <f>N32*BOM[[#This Row],[Qty]]</f>
         <v>10</v>
       </c>
     </row>
@@ -1926,7 +2009,7 @@
         <v>1E-3</v>
       </c>
       <c r="O9">
-        <f>N30*BOM[[#This Row],[Qty]]</f>
+        <f>N32*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -1969,7 +2052,7 @@
         <v>3.1E-2</v>
       </c>
       <c r="O10">
-        <f>N30*BOM[[#This Row],[Qty]]</f>
+        <f>N32*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -2012,7 +2095,7 @@
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="O11">
-        <f>N30*BOM[[#This Row],[Qty]]</f>
+        <f>N32*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -2097,7 +2180,7 @@
         <v>1.58</v>
       </c>
       <c r="O13">
-        <f>N30*BOM[[#This Row],[Qty]]</f>
+        <f>N32*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -2140,7 +2223,7 @@
         <v>1E-3</v>
       </c>
       <c r="O14">
-        <f>N30*BOM[[#This Row],[Qty]]</f>
+        <f>N32*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -2183,7 +2266,7 @@
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="O15">
-        <f>N30*BOM[[#This Row],[Qty]]</f>
+        <f>N32*BOM[[#This Row],[Qty]]</f>
         <v>10</v>
       </c>
     </row>
@@ -2226,7 +2309,7 @@
         <v>1.54</v>
       </c>
       <c r="O16">
-        <f>N30*BOM[[#This Row],[Qty]]</f>
+        <f>N32*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -2269,7 +2352,7 @@
         <v>0.20100000000000001</v>
       </c>
       <c r="O17">
-        <f>N30*BOM[[#This Row],[Qty]]</f>
+        <f>N32*BOM[[#This Row],[Qty]]</f>
         <v>15</v>
       </c>
     </row>
@@ -2312,7 +2395,7 @@
         <v>0.22</v>
       </c>
       <c r="O18">
-        <f>N30*BOM[[#This Row],[Qty]]</f>
+        <f>N32*BOM[[#This Row],[Qty]]</f>
         <v>10</v>
       </c>
     </row>
@@ -2355,7 +2438,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="O19">
-        <f>N30*BOM[[#This Row],[Qty]]</f>
+        <f>N32*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -2398,7 +2481,7 @@
         <v>0.26800000000000002</v>
       </c>
       <c r="O20">
-        <f>N30*BOM[[#This Row],[Qty]]</f>
+        <f>N32*BOM[[#This Row],[Qty]]</f>
         <v>20</v>
       </c>
     </row>
@@ -2438,7 +2521,7 @@
         <v>1.44</v>
       </c>
       <c r="O21">
-        <f>N30*BOM[[#This Row],[Qty]]</f>
+        <f>N32*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -2481,7 +2564,7 @@
         <v>1.37</v>
       </c>
       <c r="O22">
-        <f>N30*BOM[[#This Row],[Qty]]</f>
+        <f>N32*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -2527,7 +2610,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="O23">
-        <f>N30*BOM[[#This Row],[Qty]]</f>
+        <f>N32*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -2570,7 +2653,7 @@
         <v>7.87</v>
       </c>
       <c r="O24">
-        <f>N30*BOM[[#This Row],[Qty]]</f>
+        <f>N32*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -2616,7 +2699,7 @@
         <v>4.72</v>
       </c>
       <c r="O25">
-        <f>N30*BOM[[#This Row],[Qty]]</f>
+        <f>N32*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -2659,7 +2742,7 @@
         <v>2.75</v>
       </c>
       <c r="O26">
-        <f>N30*BOM[[#This Row],[Qty]]</f>
+        <f>N32*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
     </row>
@@ -2694,7 +2777,7 @@
       <c r="L27" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="M27" s="1">
+      <c r="M27" s="9">
         <v>0.69599999999999995</v>
       </c>
       <c r="N27">
@@ -2702,36 +2785,166 @@
         <v>0.69599999999999995</v>
       </c>
       <c r="O27">
-        <f>N30*BOM[[#This Row],[Qty]]</f>
+        <f>N32*BOM[[#This Row],[Qty]]</f>
         <v>5</v>
       </c>
       <c r="P27" s="1"/>
     </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>210</v>
+      </c>
+      <c r="C28" t="s">
+        <v>211</v>
+      </c>
+      <c r="D28" t="s">
+        <v>205</v>
+      </c>
+      <c r="E28" t="s">
+        <v>212</v>
+      </c>
+      <c r="F28" t="s">
+        <v>80</v>
+      </c>
+      <c r="G28" t="s">
+        <v>213</v>
+      </c>
+      <c r="H28" t="s">
+        <v>214</v>
+      </c>
+      <c r="I28" t="s">
+        <v>215</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="M28">
+        <v>0.13</v>
+      </c>
+      <c r="N28">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>0.13</v>
+      </c>
+      <c r="O28" s="7">
+        <f>N58*BOM[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+      <c r="P28" s="1"/>
+    </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
-      <c r="M29" s="5" t="s">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" t="s">
+        <v>204</v>
+      </c>
+      <c r="D29" t="s">
+        <v>205</v>
+      </c>
+      <c r="E29" t="s">
+        <v>206</v>
+      </c>
+      <c r="F29" t="s">
+        <v>80</v>
+      </c>
+      <c r="G29" t="s">
+        <v>107</v>
+      </c>
+      <c r="H29" t="s">
+        <v>207</v>
+      </c>
+      <c r="I29" t="s">
+        <v>208</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="M29" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="N29">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>0.2</v>
+      </c>
+      <c r="O29" s="7">
+        <f>N58*BOM[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="15" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>218</v>
+      </c>
+      <c r="C30" t="s">
+        <v>217</v>
+      </c>
+      <c r="D30" t="s">
+        <v>219</v>
+      </c>
+      <c r="E30" t="s">
+        <v>220</v>
+      </c>
+      <c r="F30" t="s">
+        <v>221</v>
+      </c>
+      <c r="G30" t="s">
+        <v>222</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="I30" t="s">
+        <v>224</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="M30">
+        <v>0.91</v>
+      </c>
+      <c r="N30">
+        <f>BOM[[#This Row],[Price ea.]]*BOM[[#This Row],[Qty]]</f>
+        <v>0.91</v>
+      </c>
+      <c r="O30" s="7">
+        <f>N60*BOM[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="2"/>
+      <c r="M31" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="N29" s="5">
+      <c r="N31" s="5">
         <f>SUM(BOM[Price ea. Order])</f>
-        <v>26.323</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="M30" s="5" t="s">
+        <v>27.562999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M32" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="N30" s="5">
+      <c r="N32" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="M31" s="6" t="s">
+    <row r="33" spans="13:14" x14ac:dyDescent="0.3">
+      <c r="M33" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="N31" s="5">
-        <f>N29*N30</f>
-        <v>131.61500000000001</v>
+      <c r="N33" s="5">
+        <f>N31*N32</f>
+        <v>137.815</v>
       </c>
     </row>
   </sheetData>

</xml_diff>